<commit_message>
change Config file's 'DownloadPath' to 'FileForMergePath'
</commit_message>
<xml_diff>
--- a/Data/ZXConfig.xlsx
+++ b/Data/ZXConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\Zhengxin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC430CD-C942-4125-B13A-79166A8472C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9EBE75A-8BF1-4699-9A72-357AA90754C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -253,7 +253,27 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>C:\Temp\Zhengxin\</t>
+    <t>QueueForProcessFolder</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>下载完毕所在文件夹（每次下载都会创建子文件夹）</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>直接从设备下载，未加工的文件存储位置，每次下载都会创建一个新的文件夹</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>C:\Temp\Zhengxin\DataFromDevices\</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>QueueForDeviceList</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>待读取设备队列，再下载的流程Zhengxin-Download里面使用</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -679,7 +699,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -828,11 +848,34 @@
         <v>49</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="B12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>